<commit_message>
add test is first day
</commit_message>
<xml_diff>
--- a/dataprep/维度表+维度字典.xlsx
+++ b/dataprep/维度表+维度字典.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\我的云端硬盘\work - Vova\2021 项目\2105 神策实施\6 配置文件\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Home\Developers\sa-item-setter\dataprep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67866E6C-062A-4B0C-A516-9274BBC4636E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A41CE95C-C661-44BC-9B26-409F5DAFAC97}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="19740" activeTab="2" xr2:uid="{F15D733B-B4C9-493C-A4E3-46EB06C61ACF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="19740" activeTab="4" xr2:uid="{F15D733B-B4C9-493C-A4E3-46EB06C61ACF}"/>
   </bookViews>
   <sheets>
     <sheet name="汇率表20210703" sheetId="1" r:id="rId1"/>
@@ -3141,8 +3141,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{394D0DFC-7077-45DF-B47F-B373AA107C5F}">
   <dimension ref="A1:P40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -5176,8 +5176,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35DD8817-BD5F-4250-A5E7-F1BD0972E750}">
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -5627,7 +5627,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF46C8B3-C166-4819-803A-19795B70C87B}">
   <dimension ref="A1:D594"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -14600,7 +14600,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E837C043-3014-4133-B7AB-F54C6F5003CF}">
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>

</xml_diff>